<commit_message>
correct units for pp hadron
</commit_message>
<xml_diff>
--- a/pp_hadron/expdata/20001.xlsx
+++ b/pp_hadron/expdata/20001.xlsx
@@ -70,7 +70,7 @@
     <t>count/inel</t>
   </si>
   <si>
-    <t>mb</t>
+    <t>pb</t>
   </si>
 </sst>
 </file>
@@ -78,10 +78,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -100,10 +100,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -114,9 +114,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -130,9 +130,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,9 +154,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,9 +189,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,38 +214,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -229,8 +228,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,13 +251,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +275,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,151 +407,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,17 +439,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -469,15 +463,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -489,6 +474,45 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,108 +536,84 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -622,61 +622,61 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1018,13 +1018,12 @@
   <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K2" sqref="K2:K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="2" max="3" width="10.25" customWidth="1"/>
     <col min="4" max="4" width="8.4375" style="1"/>
     <col min="10" max="10" width="9.25" customWidth="1"/>
     <col min="12" max="14" width="12.6875"/>

</xml_diff>

<commit_message>
minor updates in pp hadron
</commit_message>
<xml_diff>
--- a/pp_hadron/expdata/20001.xlsx
+++ b/pp_hadron/expdata/20001.xlsx
@@ -34,7 +34,7 @@
     <t>pt-max</t>
   </si>
   <si>
-    <t>pt</t>
+    <t>pT</t>
   </si>
   <si>
     <t>eta-min</t>
@@ -79,9 +79,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -100,6 +100,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -107,16 +115,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -130,17 +145,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,35 +162,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,30 +170,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -230,7 +186,51 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,7 +251,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,73 +413,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,91 +425,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,69 +436,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -521,7 +458,70 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,139 +544,139 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1018,7 +1018,7 @@
   <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K54"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
update key 'obs' for pp hadron
</commit_message>
<xml_diff>
--- a/pp_hadron/expdata/20001.xlsx
+++ b/pp_hadron/expdata/20001.xlsx
@@ -70,7 +70,7 @@
     <t>K+-</t>
   </si>
   <si>
-    <t>count/inel</t>
+    <t>dN/N_inel-dy-dpT</t>
   </si>
   <si>
     <t>pb</t>
@@ -81,9 +81,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -102,6 +102,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,15 +125,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -131,71 +141,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,7 +165,52 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,14 +218,22 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,7 +254,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,7 +266,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +296,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,7 +392,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,85 +404,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,43 +422,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,69 +439,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -523,8 +460,47 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -539,147 +515,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -689,12 +689,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1024,19 +1021,19 @@
   <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A54"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14"/>
   <cols>
     <col min="3" max="4" width="10.25" customWidth="1"/>
     <col min="5" max="5" width="8.4375" style="1"/>
-    <col min="11" max="11" width="9.25" customWidth="1"/>
+    <col min="11" max="11" width="16.25" customWidth="1"/>
     <col min="13" max="15" width="12.6875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1083,7 +1080,7 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1130,7 +1127,7 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1177,7 +1174,7 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1224,7 +1221,7 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1271,7 +1268,7 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1318,7 +1315,7 @@
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1365,7 +1362,7 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1412,7 +1409,7 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1459,7 +1456,7 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1506,7 +1503,7 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1553,7 +1550,7 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1600,7 +1597,7 @@
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1647,7 +1644,7 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1694,7 +1691,7 @@
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1741,7 +1738,7 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1788,7 +1785,7 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1835,7 +1832,7 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1882,7 +1879,7 @@
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1929,7 +1926,7 @@
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1976,7 +1973,7 @@
       </c>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2023,7 +2020,7 @@
       </c>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2070,7 +2067,7 @@
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2117,7 +2114,7 @@
       </c>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2164,7 +2161,7 @@
       </c>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2211,7 +2208,7 @@
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2258,7 +2255,7 @@
       </c>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2305,7 +2302,7 @@
       </c>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2352,7 +2349,7 @@
       </c>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2399,7 +2396,7 @@
       </c>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2446,7 +2443,7 @@
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2493,7 +2490,7 @@
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2540,7 +2537,7 @@
       </c>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2587,7 +2584,7 @@
       </c>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2634,7 +2631,7 @@
       </c>
     </row>
     <row r="35" spans="1:15">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2681,7 +2678,7 @@
       </c>
     </row>
     <row r="36" spans="1:15">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2728,7 +2725,7 @@
       </c>
     </row>
     <row r="37" spans="1:15">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2775,7 +2772,7 @@
       </c>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2814,7 +2811,7 @@
       <c r="M38" s="1">
         <v>0.0014294</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N38" s="2">
         <v>1.3245e-5</v>
       </c>
       <c r="O38" s="1">
@@ -2822,7 +2819,7 @@
       </c>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -2861,7 +2858,7 @@
       <c r="M39" s="1">
         <v>0.00082758</v>
       </c>
-      <c r="N39" s="3">
+      <c r="N39" s="2">
         <v>9.8267e-6</v>
       </c>
       <c r="O39" s="1">
@@ -2869,7 +2866,7 @@
       </c>
     </row>
     <row r="40" spans="1:15">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2908,15 +2905,15 @@
       <c r="M40" s="1">
         <v>0.00050668</v>
       </c>
-      <c r="N40" s="3">
+      <c r="N40" s="2">
         <v>7.6432e-6</v>
       </c>
-      <c r="O40" s="3">
+      <c r="O40" s="2">
         <v>2.8067e-5</v>
       </c>
     </row>
     <row r="41" spans="1:15">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2955,15 +2952,15 @@
       <c r="M41" s="1">
         <v>0.00032519</v>
       </c>
-      <c r="N41" s="3">
+      <c r="N41" s="2">
         <v>6.0262e-6</v>
       </c>
-      <c r="O41" s="3">
+      <c r="O41" s="2">
         <v>1.6793e-5</v>
       </c>
     </row>
     <row r="42" spans="1:15">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -3002,15 +2999,15 @@
       <c r="M42" s="1">
         <v>0.0002123</v>
       </c>
-      <c r="N42" s="3">
+      <c r="N42" s="2">
         <v>4.6342e-6</v>
       </c>
-      <c r="O42" s="3">
+      <c r="O42" s="2">
         <v>1.0574e-5</v>
       </c>
     </row>
     <row r="43" spans="1:15">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -3049,15 +3046,15 @@
       <c r="M43" s="1">
         <v>0.00014632</v>
       </c>
-      <c r="N43" s="3">
+      <c r="N43" s="2">
         <v>3.8899e-6</v>
       </c>
-      <c r="O43" s="3">
+      <c r="O43" s="2">
         <v>6.985e-6</v>
       </c>
     </row>
     <row r="44" spans="1:15">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -3096,15 +3093,15 @@
       <c r="M44" s="1">
         <v>8.5525e-5</v>
       </c>
-      <c r="N44" s="3">
+      <c r="N44" s="2">
         <v>2.1914e-6</v>
       </c>
-      <c r="O44" s="3">
+      <c r="O44" s="2">
         <v>4.1239e-6</v>
       </c>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -3143,15 +3140,15 @@
       <c r="M45" s="1">
         <v>4.7108e-5</v>
       </c>
-      <c r="N45" s="3">
+      <c r="N45" s="2">
         <v>1.6803e-6</v>
       </c>
-      <c r="O45" s="3">
+      <c r="O45" s="2">
         <v>3.9418e-6</v>
       </c>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -3187,18 +3184,18 @@
       <c r="L46" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M46" s="3">
+      <c r="M46" s="2">
         <v>2.6202e-5</v>
       </c>
-      <c r="N46" s="3">
+      <c r="N46" s="2">
         <v>1.2284e-6</v>
       </c>
-      <c r="O46" s="3">
+      <c r="O46" s="2">
         <v>2.2015e-6</v>
       </c>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -3234,18 +3231,18 @@
       <c r="L47" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M47" s="3">
+      <c r="M47" s="2">
         <v>1.5844e-5</v>
       </c>
-      <c r="N47" s="3">
+      <c r="N47" s="2">
         <v>9.2809e-7</v>
       </c>
-      <c r="O47" s="3">
+      <c r="O47" s="2">
         <v>1.3658e-6</v>
       </c>
     </row>
     <row r="48" spans="1:15">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -3281,18 +3278,18 @@
       <c r="L48" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M48" s="3">
+      <c r="M48" s="2">
         <v>1.0623e-5</v>
       </c>
-      <c r="N48" s="3">
+      <c r="N48" s="2">
         <v>7.7337e-7</v>
       </c>
-      <c r="O48" s="3">
+      <c r="O48" s="2">
         <v>9.2029e-7</v>
       </c>
     </row>
     <row r="49" spans="1:15">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -3328,18 +3325,18 @@
       <c r="L49" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M49" s="3">
+      <c r="M49" s="2">
         <v>6.7132e-6</v>
       </c>
-      <c r="N49" s="3">
+      <c r="N49" s="2">
         <v>6.5568e-7</v>
       </c>
-      <c r="O49" s="3">
+      <c r="O49" s="2">
         <v>5.8591e-7</v>
       </c>
     </row>
     <row r="50" spans="1:15">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -3375,18 +3372,18 @@
       <c r="L50" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M50" s="3">
+      <c r="M50" s="2">
         <v>4.426e-6</v>
       </c>
-      <c r="N50" s="3">
+      <c r="N50" s="2">
         <v>5.5163e-7</v>
       </c>
-      <c r="O50" s="3">
+      <c r="O50" s="2">
         <v>3.884e-7</v>
       </c>
     </row>
     <row r="51" spans="1:15">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -3422,18 +3419,18 @@
       <c r="L51" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M51" s="3">
+      <c r="M51" s="2">
         <v>3.1718e-6</v>
       </c>
-      <c r="N51" s="3">
+      <c r="N51" s="2">
         <v>4.6202e-7</v>
       </c>
-      <c r="O51" s="3">
+      <c r="O51" s="2">
         <v>2.8032e-7</v>
       </c>
     </row>
     <row r="52" spans="1:15">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -3469,18 +3466,18 @@
       <c r="L52" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M52" s="3">
+      <c r="M52" s="2">
         <v>2.1966e-6</v>
       </c>
-      <c r="N52" s="3">
+      <c r="N52" s="2">
         <v>3.4371e-7</v>
       </c>
-      <c r="O52" s="3">
+      <c r="O52" s="2">
         <v>1.9563e-7</v>
       </c>
     </row>
     <row r="53" spans="1:15">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -3516,18 +3513,18 @@
       <c r="L53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M53" s="3">
+      <c r="M53" s="2">
         <v>1.5121e-6</v>
       </c>
-      <c r="N53" s="3">
+      <c r="N53" s="2">
         <v>2.2042e-7</v>
       </c>
-      <c r="O53" s="3">
+      <c r="O53" s="2">
         <v>1.3672e-7</v>
       </c>
     </row>
     <row r="54" spans="1:15">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -3563,13 +3560,13 @@
       <c r="L54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M54" s="3">
+      <c r="M54" s="2">
         <v>8.4518e-7</v>
       </c>
-      <c r="N54" s="3">
+      <c r="N54" s="2">
         <v>1.8536e-7</v>
       </c>
-      <c r="O54" s="3">
+      <c r="O54" s="2">
         <v>7.7673e-8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add more data for pp hadron
</commit_message>
<xml_diff>
--- a/pp_hadron/expdata/20001.xlsx
+++ b/pp_hadron/expdata/20001.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17240"/>
+    <workbookView windowHeight="17540"/>
   </bookViews>
   <sheets>
-    <sheet name="HEPData-ins1797443-v1-Table_2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="20">
   <si>
     <t>idx</t>
   </si>
@@ -61,16 +61,16 @@
     <t>sys_u</t>
   </si>
   <si>
-    <t>alice</t>
+    <t>ALICE</t>
   </si>
   <si>
     <t>pp</t>
   </si>
   <si>
-    <t>K+-</t>
+    <t>kaon_+-</t>
   </si>
   <si>
-    <t>dN/N_inel-dy-dpT</t>
+    <t>dN/2-pi-pT-N_inel-dy-dpT</t>
   </si>
   <si>
     <t>pb</t>
@@ -81,10 +81,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -96,7 +96,53 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -104,7 +150,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,13 +171,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -133,23 +179,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -157,17 +188,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -178,24 +201,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,30 +225,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,13 +248,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,7 +350,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,13 +362,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,19 +380,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,85 +416,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,19 +428,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,35 +442,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,6 +462,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,6 +498,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -516,26 +516,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,159 +544,156 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -717,39 +714,39 @@
     <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
     <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
-    <cellStyle name="Bad" xfId="22" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
-    <cellStyle name="Total" xfId="24" builtinId="25"/>
-    <cellStyle name="Output" xfId="25" builtinId="21"/>
-    <cellStyle name="Currency" xfId="26" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
-    <cellStyle name="Note" xfId="28" builtinId="10"/>
-    <cellStyle name="Input" xfId="29" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
-    <cellStyle name="Good" xfId="32" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="Title" xfId="38" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
-    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
-    <cellStyle name="Link" xfId="43" builtinId="8"/>
-    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
-    <cellStyle name="Comma" xfId="45" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1016,19 +1013,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="4" width="10.25" customWidth="1"/>
-    <col min="5" max="5" width="8.4375" style="1"/>
-    <col min="11" max="11" width="16.25" customWidth="1"/>
+    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="4" max="4" width="10.5625" customWidth="1"/>
+    <col min="11" max="11" width="23.5" customWidth="1"/>
+    <col min="12" max="12" width="6.6328125" customWidth="1"/>
     <col min="13" max="15" width="12.6875"/>
   </cols>
   <sheetData>
@@ -1093,7 +1091,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F2" s="1">
         <v>0.2</v>
@@ -1105,10 +1103,10 @@
         <v>0.225</v>
       </c>
       <c r="I2" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J2" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>18</v>
@@ -1117,13 +1115,13 @@
         <v>19</v>
       </c>
       <c r="M2" s="1">
-        <v>0.51568</v>
+        <v>0.3416</v>
       </c>
       <c r="N2" s="1">
-        <v>0.00080657</v>
+        <v>0.00154</v>
       </c>
       <c r="O2" s="1">
-        <v>0.023802</v>
+        <v>0.03135</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1140,7 +1138,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F3" s="1">
         <v>0.25</v>
@@ -1152,10 +1150,10 @@
         <v>0.275</v>
       </c>
       <c r="I3" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J3" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>18</v>
@@ -1164,13 +1162,13 @@
         <v>19</v>
       </c>
       <c r="M3" s="1">
-        <v>0.5593</v>
+        <v>0.3019</v>
       </c>
       <c r="N3" s="1">
-        <v>0.00065253</v>
+        <v>0.001065</v>
       </c>
       <c r="O3" s="1">
-        <v>0.024019</v>
+        <v>0.02006</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1187,7 +1185,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F4" s="1">
         <v>0.3</v>
@@ -1199,10 +1197,10 @@
         <v>0.324999999999999</v>
       </c>
       <c r="I4" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J4" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>18</v>
@@ -1211,13 +1209,13 @@
         <v>19</v>
       </c>
       <c r="M4" s="1">
-        <v>0.59112</v>
+        <v>0.2619</v>
       </c>
       <c r="N4" s="1">
-        <v>0.0016426</v>
+        <v>0.0008301</v>
       </c>
       <c r="O4" s="1">
-        <v>0.015955</v>
+        <v>0.01056</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1234,7 +1232,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F5" s="1">
         <v>0.35</v>
@@ -1246,10 +1244,10 @@
         <v>0.375</v>
       </c>
       <c r="I5" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J5" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>18</v>
@@ -1258,13 +1256,13 @@
         <v>19</v>
       </c>
       <c r="M5" s="1">
-        <v>0.60224</v>
+        <v>0.2266</v>
       </c>
       <c r="N5" s="1">
-        <v>0.0015274</v>
+        <v>0.0006742</v>
       </c>
       <c r="O5" s="1">
-        <v>0.012826</v>
+        <v>0.007917</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1281,7 +1279,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F6" s="1">
         <v>0.4</v>
@@ -1293,10 +1291,10 @@
         <v>0.425</v>
       </c>
       <c r="I6" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J6" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>18</v>
@@ -1305,13 +1303,13 @@
         <v>19</v>
       </c>
       <c r="M6" s="1">
-        <v>0.5869</v>
+        <v>0.1957</v>
       </c>
       <c r="N6" s="1">
-        <v>0.0014041</v>
+        <v>0.0006019</v>
       </c>
       <c r="O6" s="1">
-        <v>0.011192</v>
+        <v>0.006929</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1328,7 +1326,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F7" s="1">
         <v>0.45</v>
@@ -1340,10 +1338,10 @@
         <v>0.475</v>
       </c>
       <c r="I7" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J7" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>18</v>
@@ -1352,13 +1350,13 @@
         <v>19</v>
       </c>
       <c r="M7" s="1">
-        <v>0.57798</v>
+        <v>0.1699</v>
       </c>
       <c r="N7" s="1">
-        <v>0.0083174</v>
+        <v>0.0005345</v>
       </c>
       <c r="O7" s="1">
-        <v>0.020625</v>
+        <v>0.006024</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1375,7 +1373,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F8" s="1">
         <v>0.5</v>
@@ -1387,10 +1385,10 @@
         <v>0.525</v>
       </c>
       <c r="I8" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J8" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>18</v>
@@ -1399,13 +1397,13 @@
         <v>19</v>
       </c>
       <c r="M8" s="1">
-        <v>0.54549</v>
+        <v>0.1427</v>
       </c>
       <c r="N8" s="1">
-        <v>0.0092601</v>
+        <v>0.0005154</v>
       </c>
       <c r="O8" s="1">
-        <v>0.021137</v>
+        <v>0.005581</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1422,7 +1420,7 @@
         <v>17</v>
       </c>
       <c r="E9" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F9" s="1">
         <v>0.55</v>
@@ -1434,10 +1432,10 @@
         <v>0.575</v>
       </c>
       <c r="I9" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J9" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>18</v>
@@ -1446,13 +1444,13 @@
         <v>19</v>
       </c>
       <c r="M9" s="1">
-        <v>0.51411</v>
+        <v>0.122</v>
       </c>
       <c r="N9" s="1">
-        <v>0.012247</v>
+        <v>0.0007792</v>
       </c>
       <c r="O9" s="1">
-        <v>0.023625</v>
+        <v>0.008203</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1469,7 +1467,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F10" s="1">
         <v>0.6</v>
@@ -1481,10 +1479,10 @@
         <v>0.625</v>
       </c>
       <c r="I10" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J10" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>18</v>
@@ -1493,13 +1491,13 @@
         <v>19</v>
       </c>
       <c r="M10" s="1">
-        <v>0.47246</v>
+        <v>0.1054</v>
       </c>
       <c r="N10" s="1">
-        <v>0.019924</v>
+        <v>0.0006412</v>
       </c>
       <c r="O10" s="1">
-        <v>0.028668</v>
+        <v>0.007512</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1516,7 +1514,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F11" s="1">
         <v>0.65</v>
@@ -1528,10 +1526,10 @@
         <v>0.675</v>
       </c>
       <c r="I11" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J11" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>18</v>
@@ -1540,13 +1538,13 @@
         <v>19</v>
       </c>
       <c r="M11" s="1">
-        <v>0.42735</v>
+        <v>0.08874</v>
       </c>
       <c r="N11" s="1">
-        <v>0.0030602</v>
+        <v>0.000543</v>
       </c>
       <c r="O11" s="1">
-        <v>0.010367</v>
+        <v>0.006346</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1563,7 +1561,7 @@
         <v>17</v>
       </c>
       <c r="E12" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F12" s="1">
         <v>0.7</v>
@@ -1575,10 +1573,10 @@
         <v>0.725</v>
       </c>
       <c r="I12" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J12" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>18</v>
@@ -1587,13 +1585,13 @@
         <v>19</v>
       </c>
       <c r="M12" s="1">
-        <v>0.384</v>
+        <v>0.07535</v>
       </c>
       <c r="N12" s="1">
-        <v>0.0024923</v>
+        <v>0.0004989</v>
       </c>
       <c r="O12" s="1">
-        <v>0.0088397</v>
+        <v>0.005392</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1610,7 +1608,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F13" s="1">
         <v>0.75</v>
@@ -1622,10 +1620,10 @@
         <v>0.775</v>
       </c>
       <c r="I13" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J13" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>18</v>
@@ -1634,13 +1632,13 @@
         <v>19</v>
       </c>
       <c r="M13" s="1">
-        <v>0.34841</v>
+        <v>0.06347</v>
       </c>
       <c r="N13" s="1">
-        <v>0.0020981</v>
+        <v>0.0003828</v>
       </c>
       <c r="O13" s="1">
-        <v>0.007632</v>
+        <v>0.004564</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1657,7 +1655,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F14" s="1">
         <v>0.8</v>
@@ -1669,10 +1667,10 @@
         <v>0.825</v>
       </c>
       <c r="I14" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J14" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>18</v>
@@ -1681,13 +1679,13 @@
         <v>19</v>
       </c>
       <c r="M14" s="1">
-        <v>0.31736</v>
+        <v>0.05376</v>
       </c>
       <c r="N14" s="1">
-        <v>0.0019195</v>
+        <v>0.0003436</v>
       </c>
       <c r="O14" s="1">
-        <v>0.0069163</v>
+        <v>0.003866</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1704,7 +1702,7 @@
         <v>17</v>
       </c>
       <c r="E15" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F15" s="1">
         <v>0.85</v>
@@ -1716,10 +1714,10 @@
         <v>0.875</v>
       </c>
       <c r="I15" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J15" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>18</v>
@@ -1728,13 +1726,13 @@
         <v>19</v>
       </c>
       <c r="M15" s="1">
-        <v>0.28837</v>
+        <v>0.0456</v>
       </c>
       <c r="N15" s="1">
-        <v>0.0017446</v>
+        <v>0.0003475</v>
       </c>
       <c r="O15" s="1">
-        <v>0.0062002</v>
+        <v>0.003286</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1751,7 +1749,7 @@
         <v>17</v>
       </c>
       <c r="E16" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F16" s="1">
         <v>0.9</v>
@@ -1763,10 +1761,10 @@
         <v>0.925</v>
       </c>
       <c r="I16" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J16" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>18</v>
@@ -1775,13 +1773,13 @@
         <v>19</v>
       </c>
       <c r="M16" s="1">
-        <v>0.25961</v>
+        <v>0.03886</v>
       </c>
       <c r="N16" s="1">
-        <v>0.0015909</v>
+        <v>0.0003066</v>
       </c>
       <c r="O16" s="1">
-        <v>0.0055925</v>
+        <v>0.002807</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1798,7 +1796,7 @@
         <v>17</v>
       </c>
       <c r="E17" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F17" s="1">
         <v>0.95</v>
@@ -1810,10 +1808,10 @@
         <v>0.975</v>
       </c>
       <c r="I17" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J17" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>18</v>
@@ -1822,13 +1820,13 @@
         <v>19</v>
       </c>
       <c r="M17" s="1">
-        <v>0.23219</v>
+        <v>0.03289</v>
       </c>
       <c r="N17" s="1">
-        <v>0.001439</v>
+        <v>0.0002632</v>
       </c>
       <c r="O17" s="1">
-        <v>0.0049711</v>
+        <v>0.002383</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1845,7 +1843,7 @@
         <v>17</v>
       </c>
       <c r="E18" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -1857,10 +1855,10 @@
         <v>1.05</v>
       </c>
       <c r="I18" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J18" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>18</v>
@@ -1869,13 +1867,13 @@
         <v>19</v>
       </c>
       <c r="M18" s="1">
-        <v>0.1985</v>
+        <v>0.0258</v>
       </c>
       <c r="N18" s="1">
-        <v>0.0011015</v>
+        <v>0.0001714</v>
       </c>
       <c r="O18" s="1">
-        <v>0.0042194</v>
+        <v>0.00188</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1892,7 +1890,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F19" s="1">
         <v>1.1</v>
@@ -1904,10 +1902,10 @@
         <v>1.15</v>
       </c>
       <c r="I19" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J19" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>18</v>
@@ -1916,13 +1914,13 @@
         <v>19</v>
       </c>
       <c r="M19" s="1">
-        <v>0.16249</v>
+        <v>0.01894</v>
       </c>
       <c r="N19" s="1">
-        <v>0.0008998</v>
+        <v>0.0001449</v>
       </c>
       <c r="O19" s="1">
-        <v>0.0033849</v>
+        <v>0.001397</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1939,7 +1937,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F20" s="1">
         <v>1.2</v>
@@ -1951,10 +1949,10 @@
         <v>1.25</v>
       </c>
       <c r="I20" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J20" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>18</v>
@@ -1963,13 +1961,13 @@
         <v>19</v>
       </c>
       <c r="M20" s="1">
-        <v>0.13269</v>
+        <v>0.01419</v>
       </c>
       <c r="N20" s="1">
-        <v>0.0008134</v>
+        <v>0.0001368</v>
       </c>
       <c r="O20" s="1">
-        <v>0.0028729</v>
+        <v>0.00109</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1986,7 +1984,7 @@
         <v>17</v>
       </c>
       <c r="E21" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F21" s="1">
         <v>1.3</v>
@@ -1998,10 +1996,10 @@
         <v>1.35</v>
       </c>
       <c r="I21" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J21" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>18</v>
@@ -2010,13 +2008,13 @@
         <v>19</v>
       </c>
       <c r="M21" s="1">
-        <v>0.10961</v>
+        <v>0.01055</v>
       </c>
       <c r="N21" s="1">
-        <v>0.00067058</v>
+        <v>0.0001118</v>
       </c>
       <c r="O21" s="1">
-        <v>0.0023412</v>
+        <v>0.0008315</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -2033,7 +2031,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F22" s="1">
         <v>1.4</v>
@@ -2045,10 +2043,10 @@
         <v>1.45</v>
       </c>
       <c r="I22" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J22" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>18</v>
@@ -2057,13 +2055,13 @@
         <v>19</v>
       </c>
       <c r="M22" s="1">
-        <v>0.090705</v>
+        <v>0.008014</v>
       </c>
       <c r="N22" s="1">
-        <v>0.00052204</v>
+        <v>9.343e-5</v>
       </c>
       <c r="O22" s="1">
-        <v>0.0018101</v>
+        <v>0.0006634</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -2080,7 +2078,7 @@
         <v>17</v>
       </c>
       <c r="E23" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F23" s="1">
         <v>1.5</v>
@@ -2092,10 +2090,10 @@
         <v>1.55</v>
       </c>
       <c r="I23" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J23" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>18</v>
@@ -2104,13 +2102,13 @@
         <v>19</v>
       </c>
       <c r="M23" s="1">
-        <v>0.076391</v>
+        <v>0.006078</v>
       </c>
       <c r="N23" s="1">
-        <v>0.00048652</v>
+        <v>5.325e-5</v>
       </c>
       <c r="O23" s="1">
-        <v>0.0015257</v>
+        <v>0.000375</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -2127,7 +2125,7 @@
         <v>17</v>
       </c>
       <c r="E24" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F24" s="1">
         <v>1.6</v>
@@ -2139,10 +2137,10 @@
         <v>1.65</v>
       </c>
       <c r="I24" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J24" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>18</v>
@@ -2151,13 +2149,13 @@
         <v>19</v>
       </c>
       <c r="M24" s="1">
-        <v>0.063961</v>
+        <v>0.004621</v>
       </c>
       <c r="N24" s="1">
-        <v>0.00041419</v>
+        <v>4.491e-5</v>
       </c>
       <c r="O24" s="1">
-        <v>0.001255</v>
+        <v>0.0002782</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -2174,7 +2172,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F25" s="1">
         <v>1.7</v>
@@ -2186,10 +2184,10 @@
         <v>1.75</v>
       </c>
       <c r="I25" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J25" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>18</v>
@@ -2198,13 +2196,13 @@
         <v>19</v>
       </c>
       <c r="M25" s="1">
-        <v>0.053464</v>
+        <v>0.003636</v>
       </c>
       <c r="N25" s="1">
-        <v>0.0005304</v>
+        <v>3.812e-5</v>
       </c>
       <c r="O25" s="1">
-        <v>0.001343</v>
+        <v>0.0002335</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -2221,7 +2219,7 @@
         <v>17</v>
       </c>
       <c r="E26" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F26" s="1">
         <v>1.8</v>
@@ -2233,10 +2231,10 @@
         <v>1.85</v>
       </c>
       <c r="I26" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J26" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>18</v>
@@ -2245,13 +2243,13 @@
         <v>19</v>
       </c>
       <c r="M26" s="1">
-        <v>0.045386</v>
+        <v>0.002827</v>
       </c>
       <c r="N26" s="1">
-        <v>0.00064914</v>
+        <v>3.288e-5</v>
       </c>
       <c r="O26" s="1">
-        <v>0.0014144</v>
+        <v>0.0001786</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -2268,7 +2266,7 @@
         <v>17</v>
       </c>
       <c r="E27" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F27" s="1">
         <v>1.9</v>
@@ -2280,10 +2278,10 @@
         <v>1.95</v>
       </c>
       <c r="I27" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J27" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>18</v>
@@ -2292,13 +2290,13 @@
         <v>19</v>
       </c>
       <c r="M27" s="1">
-        <v>0.037751</v>
+        <v>0.002233</v>
       </c>
       <c r="N27" s="1">
-        <v>0.00067277</v>
+        <v>2.828e-5</v>
       </c>
       <c r="O27" s="1">
-        <v>0.0013045</v>
+        <v>0.0001484</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -2315,22 +2313,22 @@
         <v>17</v>
       </c>
       <c r="E28" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
       </c>
       <c r="G28" s="1">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="H28" s="1">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
       <c r="I28" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J28" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>18</v>
@@ -2339,13 +2337,13 @@
         <v>19</v>
       </c>
       <c r="M28" s="1">
-        <v>0.028729</v>
+        <v>0.001839</v>
       </c>
       <c r="N28" s="1">
-        <v>0.00057405</v>
+        <v>2.454e-5</v>
       </c>
       <c r="O28" s="1">
-        <v>0.0011411</v>
+        <v>0.0001263</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -2362,22 +2360,22 @@
         <v>17</v>
       </c>
       <c r="E29" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F29" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="G29" s="1">
         <v>2.2</v>
       </c>
-      <c r="G29" s="1">
-        <v>2.4</v>
-      </c>
       <c r="H29" s="1">
-        <v>2.3</v>
+        <v>2.15</v>
       </c>
       <c r="I29" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J29" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>18</v>
@@ -2386,13 +2384,13 @@
         <v>19</v>
       </c>
       <c r="M29" s="1">
-        <v>0.020563</v>
+        <v>0.001395</v>
       </c>
       <c r="N29" s="1">
-        <v>0.00048974</v>
+        <v>2.164e-5</v>
       </c>
       <c r="O29" s="1">
-        <v>0.000897</v>
+        <v>8.966e-5</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -2409,22 +2407,22 @@
         <v>17</v>
       </c>
       <c r="E30" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F30" s="1">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="G30" s="1">
-        <v>2.6</v>
+        <v>2.3</v>
       </c>
       <c r="H30" s="1">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="I30" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J30" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>18</v>
@@ -2433,13 +2431,13 @@
         <v>19</v>
       </c>
       <c r="M30" s="1">
-        <v>0.014631</v>
+        <v>0.001148</v>
       </c>
       <c r="N30" s="1">
-        <v>0.00035623</v>
+        <v>1.832e-5</v>
       </c>
       <c r="O30" s="1">
-        <v>0.00061022</v>
+        <v>8.62e-5</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -2456,22 +2454,22 @@
         <v>17</v>
       </c>
       <c r="E31" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F31" s="1">
-        <v>2.6</v>
+        <v>2.3</v>
       </c>
       <c r="G31" s="1">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="H31" s="1">
-        <v>2.7</v>
+        <v>2.34999999999999</v>
       </c>
       <c r="I31" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J31" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>18</v>
@@ -2480,13 +2478,13 @@
         <v>19</v>
       </c>
       <c r="M31" s="1">
-        <v>0.010764</v>
+        <v>0.0008884</v>
       </c>
       <c r="N31" s="1">
-        <v>0.00028068</v>
+        <v>1.59e-5</v>
       </c>
       <c r="O31" s="1">
-        <v>0.00045366</v>
+        <v>6.565e-5</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2503,22 +2501,22 @@
         <v>17</v>
       </c>
       <c r="E32" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F32" s="1">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="G32" s="1">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="H32" s="1">
-        <v>2.9</v>
+        <v>2.45</v>
       </c>
       <c r="I32" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J32" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>18</v>
@@ -2527,13 +2525,13 @@
         <v>19</v>
       </c>
       <c r="M32" s="1">
-        <v>0.0079173</v>
+        <v>0.0007249</v>
       </c>
       <c r="N32" s="1">
-        <v>0.00023113</v>
+        <v>1.71e-5</v>
       </c>
       <c r="O32" s="1">
-        <v>0.00035523</v>
+        <v>5.965e-5</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -2550,22 +2548,22 @@
         <v>17</v>
       </c>
       <c r="E33" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F33" s="1">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="G33" s="1">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="H33" s="1">
-        <v>3.1</v>
+        <v>2.55</v>
       </c>
       <c r="I33" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J33" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>18</v>
@@ -2574,13 +2572,13 @@
         <v>19</v>
       </c>
       <c r="M33" s="1">
-        <v>0.0058669</v>
+        <v>0.0005741</v>
       </c>
       <c r="N33" s="1">
-        <v>0.00015369</v>
+        <v>1.473e-5</v>
       </c>
       <c r="O33" s="1">
-        <v>0.00030367</v>
+        <v>4.933e-5</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -2597,22 +2595,22 @@
         <v>17</v>
       </c>
       <c r="E34" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F34" s="1">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="G34" s="1">
-        <v>3.4</v>
+        <v>2.7</v>
       </c>
       <c r="H34" s="1">
-        <v>3.3</v>
+        <v>2.65</v>
       </c>
       <c r="I34" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J34" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>18</v>
@@ -2621,13 +2619,13 @@
         <v>19</v>
       </c>
       <c r="M34" s="1">
-        <v>0.0044239</v>
+        <v>0.0004736</v>
       </c>
       <c r="N34" s="1">
-        <v>0.00012063</v>
+        <v>1.311e-5</v>
       </c>
       <c r="O34" s="1">
-        <v>0.00024061</v>
+        <v>4.244e-5</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -2644,22 +2642,22 @@
         <v>17</v>
       </c>
       <c r="E35" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F35" s="1">
-        <v>3.4</v>
+        <v>2.7</v>
       </c>
       <c r="G35" s="1">
-        <v>3.6</v>
+        <v>2.8</v>
       </c>
       <c r="H35" s="1">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="I35" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J35" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>18</v>
@@ -2668,13 +2666,13 @@
         <v>19</v>
       </c>
       <c r="M35" s="1">
-        <v>0.003417</v>
+        <v>0.0003819</v>
       </c>
       <c r="N35" s="1">
-        <v>9.5916e-5</v>
+        <v>1.154e-5</v>
       </c>
       <c r="O35" s="1">
-        <v>0.00020466</v>
+        <v>3.687e-5</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2691,22 +2689,22 @@
         <v>17</v>
       </c>
       <c r="E36" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F36" s="1">
-        <v>3.6</v>
+        <v>2.8</v>
       </c>
       <c r="G36" s="1">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="H36" s="1">
-        <v>3.7</v>
+        <v>2.84999999999999</v>
       </c>
       <c r="I36" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J36" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>18</v>
@@ -2715,13 +2713,13 @@
         <v>19</v>
       </c>
       <c r="M36" s="1">
-        <v>0.0026276</v>
+        <v>0.0003264</v>
       </c>
       <c r="N36" s="1">
-        <v>7.1774e-5</v>
+        <v>1.105e-5</v>
       </c>
       <c r="O36" s="1">
-        <v>0.00016301</v>
+        <v>2.993e-5</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -2738,22 +2736,22 @@
         <v>17</v>
       </c>
       <c r="E37" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F37" s="1">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="G37" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H37" s="1">
-        <v>3.9</v>
+        <v>2.95</v>
       </c>
       <c r="I37" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J37" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>18</v>
@@ -2762,13 +2760,13 @@
         <v>19</v>
       </c>
       <c r="M37" s="1">
-        <v>0.0020607</v>
+        <v>0.0002662</v>
       </c>
       <c r="N37" s="1">
-        <v>5.3989e-5</v>
+        <v>8.725e-6</v>
       </c>
       <c r="O37" s="1">
-        <v>0.00013189</v>
+        <v>2.552e-5</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -2785,22 +2783,22 @@
         <v>17</v>
       </c>
       <c r="E38" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F38" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G38" s="1">
-        <v>4.5</v>
+        <v>3.2</v>
       </c>
       <c r="H38" s="1">
-        <v>4.25</v>
+        <v>3.1</v>
       </c>
       <c r="I38" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J38" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>18</v>
@@ -2809,13 +2807,13 @@
         <v>19</v>
       </c>
       <c r="M38" s="1">
-        <v>0.0014294</v>
-      </c>
-      <c r="N38" s="2">
-        <v>1.3245e-5</v>
+        <v>0.0001962</v>
+      </c>
+      <c r="N38" s="1">
+        <v>5.745e-6</v>
       </c>
       <c r="O38" s="1">
-        <v>9.3738e-5</v>
+        <v>1.789e-5</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -2832,22 +2830,22 @@
         <v>17</v>
       </c>
       <c r="E39" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F39" s="1">
-        <v>4.5</v>
+        <v>3.2</v>
       </c>
       <c r="G39" s="1">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="H39" s="1">
-        <v>4.75</v>
+        <v>3.3</v>
       </c>
       <c r="I39" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J39" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>18</v>
@@ -2856,13 +2854,13 @@
         <v>19</v>
       </c>
       <c r="M39" s="1">
-        <v>0.00082758</v>
-      </c>
-      <c r="N39" s="2">
-        <v>9.8267e-6</v>
+        <v>0.0001392</v>
+      </c>
+      <c r="N39" s="1">
+        <v>3.693e-6</v>
       </c>
       <c r="O39" s="1">
-        <v>4.913e-5</v>
+        <v>1.193e-5</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -2879,22 +2877,22 @@
         <v>17</v>
       </c>
       <c r="E40" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F40" s="1">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="G40" s="1">
-        <v>5.5</v>
+        <v>3.6</v>
       </c>
       <c r="H40" s="1">
-        <v>5.25</v>
+        <v>3.5</v>
       </c>
       <c r="I40" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J40" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>18</v>
@@ -2903,13 +2901,13 @@
         <v>19</v>
       </c>
       <c r="M40" s="1">
-        <v>0.00050668</v>
-      </c>
-      <c r="N40" s="2">
-        <v>7.6432e-6</v>
-      </c>
-      <c r="O40" s="2">
-        <v>2.8067e-5</v>
+        <v>9.704e-5</v>
+      </c>
+      <c r="N40" s="1">
+        <v>2.432e-6</v>
+      </c>
+      <c r="O40" s="1">
+        <v>8.336e-6</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -2926,22 +2924,22 @@
         <v>17</v>
       </c>
       <c r="E41" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F41" s="1">
-        <v>5.5</v>
+        <v>3.6</v>
       </c>
       <c r="G41" s="1">
-        <v>6</v>
+        <v>3.8</v>
       </c>
       <c r="H41" s="1">
-        <v>5.75</v>
+        <v>3.7</v>
       </c>
       <c r="I41" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J41" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>18</v>
@@ -2950,13 +2948,13 @@
         <v>19</v>
       </c>
       <c r="M41" s="1">
-        <v>0.00032519</v>
-      </c>
-      <c r="N41" s="2">
-        <v>6.0262e-6</v>
-      </c>
-      <c r="O41" s="2">
-        <v>1.6793e-5</v>
+        <v>7.188e-5</v>
+      </c>
+      <c r="N41" s="1">
+        <v>7.692e-7</v>
+      </c>
+      <c r="O41" s="1">
+        <v>7.839e-6</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2973,22 +2971,22 @@
         <v>17</v>
       </c>
       <c r="E42" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F42" s="1">
-        <v>6</v>
+        <v>3.8</v>
       </c>
       <c r="G42" s="1">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="H42" s="1">
-        <v>6.25</v>
+        <v>3.9</v>
       </c>
       <c r="I42" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J42" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>18</v>
@@ -2997,13 +2995,13 @@
         <v>19</v>
       </c>
       <c r="M42" s="1">
-        <v>0.0002123</v>
-      </c>
-      <c r="N42" s="2">
-        <v>4.6342e-6</v>
-      </c>
-      <c r="O42" s="2">
-        <v>1.0574e-5</v>
+        <v>5.291e-5</v>
+      </c>
+      <c r="N42" s="1">
+        <v>5.587e-7</v>
+      </c>
+      <c r="O42" s="1">
+        <v>5.512e-6</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -3020,22 +3018,22 @@
         <v>17</v>
       </c>
       <c r="E43" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F43" s="1">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="G43" s="1">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="H43" s="1">
-        <v>6.75</v>
+        <v>4.25</v>
       </c>
       <c r="I43" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J43" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>18</v>
@@ -3044,13 +3042,13 @@
         <v>19</v>
       </c>
       <c r="M43" s="1">
-        <v>0.00014632</v>
-      </c>
-      <c r="N43" s="2">
-        <v>3.8899e-6</v>
-      </c>
-      <c r="O43" s="2">
-        <v>6.985e-6</v>
+        <v>3.258e-5</v>
+      </c>
+      <c r="N43" s="1">
+        <v>3.369e-7</v>
+      </c>
+      <c r="O43" s="1">
+        <v>3.243e-6</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -3067,22 +3065,22 @@
         <v>17</v>
       </c>
       <c r="E44" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F44" s="1">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="G44" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H44" s="1">
-        <v>7.5</v>
+        <v>4.75</v>
       </c>
       <c r="I44" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J44" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>18</v>
@@ -3091,13 +3089,13 @@
         <v>19</v>
       </c>
       <c r="M44" s="1">
-        <v>8.5525e-5</v>
-      </c>
-      <c r="N44" s="2">
-        <v>2.1914e-6</v>
-      </c>
-      <c r="O44" s="2">
-        <v>4.1239e-6</v>
+        <v>1.716e-5</v>
+      </c>
+      <c r="N44" s="1">
+        <v>2.091e-7</v>
+      </c>
+      <c r="O44" s="1">
+        <v>1.624e-6</v>
       </c>
     </row>
     <row r="45" spans="1:15">
@@ -3114,22 +3112,22 @@
         <v>17</v>
       </c>
       <c r="E45" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F45" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G45" s="1">
-        <v>9</v>
+        <v>5.5</v>
       </c>
       <c r="H45" s="1">
-        <v>8.5</v>
+        <v>5.25</v>
       </c>
       <c r="I45" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J45" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>18</v>
@@ -3138,13 +3136,13 @@
         <v>19</v>
       </c>
       <c r="M45" s="1">
-        <v>4.7108e-5</v>
-      </c>
-      <c r="N45" s="2">
-        <v>1.6803e-6</v>
-      </c>
-      <c r="O45" s="2">
-        <v>3.9418e-6</v>
+        <v>9.485e-6</v>
+      </c>
+      <c r="N45" s="1">
+        <v>1.302e-7</v>
+      </c>
+      <c r="O45" s="1">
+        <v>8.894e-7</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -3161,22 +3159,22 @@
         <v>17</v>
       </c>
       <c r="E46" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F46" s="1">
-        <v>9</v>
+        <v>5.5</v>
       </c>
       <c r="G46" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H46" s="1">
-        <v>9.5</v>
+        <v>5.75</v>
       </c>
       <c r="I46" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J46" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>18</v>
@@ -3184,14 +3182,14 @@
       <c r="L46" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M46" s="2">
-        <v>2.6202e-5</v>
-      </c>
-      <c r="N46" s="2">
-        <v>1.2284e-6</v>
-      </c>
-      <c r="O46" s="2">
-        <v>2.2015e-6</v>
+      <c r="M46" s="1">
+        <v>5.389e-6</v>
+      </c>
+      <c r="N46" s="1">
+        <v>8.71e-8</v>
+      </c>
+      <c r="O46" s="1">
+        <v>4.995e-7</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -3208,22 +3206,22 @@
         <v>17</v>
       </c>
       <c r="E47" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F47" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G47" s="1">
-        <v>11</v>
+        <v>6.5</v>
       </c>
       <c r="H47" s="1">
-        <v>10.5</v>
+        <v>6.25</v>
       </c>
       <c r="I47" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J47" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>18</v>
@@ -3231,14 +3229,14 @@
       <c r="L47" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M47" s="2">
-        <v>1.5844e-5</v>
-      </c>
-      <c r="N47" s="2">
-        <v>9.2809e-7</v>
-      </c>
-      <c r="O47" s="2">
-        <v>1.3658e-6</v>
+      <c r="M47" s="1">
+        <v>3.275e-6</v>
+      </c>
+      <c r="N47" s="1">
+        <v>6.24e-8</v>
+      </c>
+      <c r="O47" s="1">
+        <v>3.202e-7</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -3255,22 +3253,22 @@
         <v>17</v>
       </c>
       <c r="E48" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F48" s="1">
-        <v>11</v>
+        <v>6.5</v>
       </c>
       <c r="G48" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H48" s="1">
-        <v>11.5</v>
+        <v>6.75</v>
       </c>
       <c r="I48" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J48" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>18</v>
@@ -3278,14 +3276,14 @@
       <c r="L48" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M48" s="2">
-        <v>1.0623e-5</v>
-      </c>
-      <c r="N48" s="2">
-        <v>7.7337e-7</v>
-      </c>
-      <c r="O48" s="2">
-        <v>9.2029e-7</v>
+      <c r="M48" s="1">
+        <v>2.082e-6</v>
+      </c>
+      <c r="N48" s="1">
+        <v>4.8e-8</v>
+      </c>
+      <c r="O48" s="1">
+        <v>2.122e-7</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -3302,22 +3300,22 @@
         <v>17</v>
       </c>
       <c r="E49" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F49" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G49" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H49" s="1">
-        <v>12.5</v>
+        <v>7.5</v>
       </c>
       <c r="I49" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J49" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>18</v>
@@ -3325,14 +3323,14 @@
       <c r="L49" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M49" s="2">
-        <v>6.7132e-6</v>
-      </c>
-      <c r="N49" s="2">
-        <v>6.5568e-7</v>
-      </c>
-      <c r="O49" s="2">
-        <v>5.8591e-7</v>
+      <c r="M49" s="1">
+        <v>1.078e-6</v>
+      </c>
+      <c r="N49" s="1">
+        <v>2.44e-8</v>
+      </c>
+      <c r="O49" s="1">
+        <v>1.096e-7</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -3349,22 +3347,22 @@
         <v>17</v>
       </c>
       <c r="E50" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F50" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G50" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H50" s="1">
-        <v>13.5</v>
+        <v>8.5</v>
       </c>
       <c r="I50" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J50" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>18</v>
@@ -3372,14 +3370,14 @@
       <c r="L50" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M50" s="2">
-        <v>4.426e-6</v>
-      </c>
-      <c r="N50" s="2">
-        <v>5.5163e-7</v>
-      </c>
-      <c r="O50" s="2">
-        <v>3.884e-7</v>
+      <c r="M50" s="1">
+        <v>4.715e-7</v>
+      </c>
+      <c r="N50" s="1">
+        <v>1.49e-8</v>
+      </c>
+      <c r="O50" s="1">
+        <v>4.84e-8</v>
       </c>
     </row>
     <row r="51" spans="1:15">
@@ -3396,22 +3394,22 @@
         <v>17</v>
       </c>
       <c r="E51" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F51" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G51" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H51" s="1">
-        <v>14.5</v>
+        <v>9.5</v>
       </c>
       <c r="I51" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J51" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>18</v>
@@ -3419,14 +3417,14 @@
       <c r="L51" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M51" s="2">
-        <v>3.1718e-6</v>
-      </c>
-      <c r="N51" s="2">
-        <v>4.6202e-7</v>
-      </c>
-      <c r="O51" s="2">
-        <v>2.8032e-7</v>
+      <c r="M51" s="1">
+        <v>2.426e-7</v>
+      </c>
+      <c r="N51" s="1">
+        <v>9.8e-9</v>
+      </c>
+      <c r="O51" s="1">
+        <v>2.45e-8</v>
       </c>
     </row>
     <row r="52" spans="1:15">
@@ -3443,22 +3441,22 @@
         <v>17</v>
       </c>
       <c r="E52" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F52" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G52" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H52" s="1">
-        <v>15.5</v>
+        <v>10.5</v>
       </c>
       <c r="I52" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J52" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>18</v>
@@ -3466,14 +3464,14 @@
       <c r="L52" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M52" s="2">
-        <v>2.1966e-6</v>
-      </c>
-      <c r="N52" s="2">
-        <v>3.4371e-7</v>
-      </c>
-      <c r="O52" s="2">
-        <v>1.9563e-7</v>
+      <c r="M52" s="1">
+        <v>1.33e-7</v>
+      </c>
+      <c r="N52" s="1">
+        <v>7.3e-9</v>
+      </c>
+      <c r="O52" s="1">
+        <v>1.33e-8</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -3490,22 +3488,22 @@
         <v>17</v>
       </c>
       <c r="E53" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F53" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G53" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H53" s="1">
-        <v>17</v>
+        <v>11.5</v>
       </c>
       <c r="I53" s="1">
-        <v>-0.5</v>
+        <v>-0.8</v>
       </c>
       <c r="J53" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>18</v>
@@ -3513,14 +3511,14 @@
       <c r="L53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M53" s="2">
-        <v>1.5121e-6</v>
-      </c>
-      <c r="N53" s="2">
-        <v>2.2042e-7</v>
-      </c>
-      <c r="O53" s="2">
-        <v>1.3672e-7</v>
+      <c r="M53" s="1">
+        <v>7.47e-8</v>
+      </c>
+      <c r="N53" s="1">
+        <v>5.1e-9</v>
+      </c>
+      <c r="O53" s="1">
+        <v>7.5e-9</v>
       </c>
     </row>
     <row r="54" spans="1:15">
@@ -3537,41 +3535,327 @@
         <v>17</v>
       </c>
       <c r="E54" s="1">
-        <v>5020</v>
+        <v>2760</v>
       </c>
       <c r="F54" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G54" s="1">
+        <v>13</v>
+      </c>
+      <c r="H54" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="I54" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M54" s="1">
+        <v>4.39e-8</v>
+      </c>
+      <c r="N54" s="1">
+        <v>3.5e-9</v>
+      </c>
+      <c r="O54" s="1">
+        <v>4.5e-9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2760</v>
+      </c>
+      <c r="F55" s="1">
+        <v>13</v>
+      </c>
+      <c r="G55" s="1">
+        <v>14</v>
+      </c>
+      <c r="H55" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="I55" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="J55" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M55" s="1">
+        <v>2.86e-8</v>
+      </c>
+      <c r="N55" s="1">
+        <v>2.8e-9</v>
+      </c>
+      <c r="O55" s="1">
+        <v>2.9e-9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="1">
+        <v>2760</v>
+      </c>
+      <c r="F56" s="1">
+        <v>14</v>
+      </c>
+      <c r="G56" s="1">
+        <v>15</v>
+      </c>
+      <c r="H56" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="I56" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M56" s="1">
+        <v>1.66e-8</v>
+      </c>
+      <c r="N56" s="1">
+        <v>1.9e-9</v>
+      </c>
+      <c r="O56" s="1">
+        <v>1.8e-9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2760</v>
+      </c>
+      <c r="F57" s="1">
+        <v>15</v>
+      </c>
+      <c r="G57" s="1">
+        <v>16</v>
+      </c>
+      <c r="H57" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="I57" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M57" s="1">
+        <v>1.05e-8</v>
+      </c>
+      <c r="N57" s="1">
+        <v>1.6e-9</v>
+      </c>
+      <c r="O57" s="1">
+        <v>1.1e-9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="1">
+        <v>2760</v>
+      </c>
+      <c r="F58" s="1">
+        <v>16</v>
+      </c>
+      <c r="G58" s="1">
+        <v>18</v>
+      </c>
+      <c r="H58" s="1">
+        <v>17</v>
+      </c>
+      <c r="I58" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="1">
+        <v>4.6e-9</v>
+      </c>
+      <c r="N58" s="1">
+        <v>9e-10</v>
+      </c>
+      <c r="O58" s="1">
+        <v>6e-10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="1">
+        <v>2760</v>
+      </c>
+      <c r="F59" s="1">
+        <v>18</v>
+      </c>
+      <c r="G59" s="1">
         <v>20</v>
       </c>
-      <c r="H54" s="1">
-        <v>19</v>
-      </c>
-      <c r="I54" s="1">
-        <v>-0.5</v>
-      </c>
-      <c r="J54" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M54" s="2">
-        <v>8.4518e-7</v>
-      </c>
-      <c r="N54" s="2">
-        <v>1.8536e-7</v>
-      </c>
-      <c r="O54" s="2">
-        <v>7.7673e-8</v>
-      </c>
+      <c r="H59" s="1">
+        <v>19</v>
+      </c>
+      <c r="I59" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="J59" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59" s="1">
+        <v>2.3e-9</v>
+      </c>
+      <c r="N59" s="1">
+        <v>6e-10</v>
+      </c>
+      <c r="O59" s="1">
+        <v>3e-10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>